<commit_message>
Added some additional county information.
</commit_message>
<xml_diff>
--- a/Data/Podaci po zupanijama.xlsx
+++ b/Data/Podaci po zupanijama.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domag\Documents\ZavrsniRad\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domagojrunjak/Documents/Zavrsni rad/zavrsni-rad/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE7D4AB-B7AB-4450-A2FA-B2BD24E20AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E2E562-7DCA-614F-A556-5BB6464FA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-3100" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Naziv županije</t>
   </si>
@@ -115,6 +115,75 @@
   </si>
   <si>
     <t>2021.</t>
+  </si>
+  <si>
+    <t>Sjedište županije</t>
+  </si>
+  <si>
+    <t>Zagreb</t>
+  </si>
+  <si>
+    <t>Sisak</t>
+  </si>
+  <si>
+    <t>Karlovac</t>
+  </si>
+  <si>
+    <t>Varaždin</t>
+  </si>
+  <si>
+    <t>Koprivnica</t>
+  </si>
+  <si>
+    <t>Bjelovar</t>
+  </si>
+  <si>
+    <t>Rijeka</t>
+  </si>
+  <si>
+    <t>Gospić</t>
+  </si>
+  <si>
+    <t>Virovitica</t>
+  </si>
+  <si>
+    <t>Požega</t>
+  </si>
+  <si>
+    <t>Slavonski Brod</t>
+  </si>
+  <si>
+    <t>Zadar</t>
+  </si>
+  <si>
+    <t>Osijek</t>
+  </si>
+  <si>
+    <t>Šibenik</t>
+  </si>
+  <si>
+    <t>Vukovar</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Pazin</t>
+  </si>
+  <si>
+    <t>Dubrovnik</t>
+  </si>
+  <si>
+    <t>Čakovec</t>
+  </si>
+  <si>
+    <t>Krapina</t>
+  </si>
+  <si>
+    <t>Površina</t>
+  </si>
+  <si>
+    <t>Gustoća naseljenosti</t>
   </si>
 </sst>
 </file>
@@ -433,652 +502,855 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>3060</v>
+      </c>
+      <c r="D2">
+        <v>98.03</v>
+      </c>
+      <c r="E2" s="1">
         <v>134754</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>194643</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>224095</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>233875</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>282989</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>309696</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>316606</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>301206</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1229</v>
+      </c>
+      <c r="D3">
+        <v>98.21</v>
+      </c>
+      <c r="E3" s="1">
         <v>100804</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>152047</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>175227</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>168952</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>148779</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>142432</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>132892</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>120942</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>4468</v>
+      </c>
+      <c r="D4">
+        <v>31.25</v>
+      </c>
+      <c r="E4" s="1">
         <v>168292</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>235514</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>268287</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>255635</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>251332</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>185387</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>172439</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>140549</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>3622</v>
+      </c>
+      <c r="D5">
+        <v>30.97</v>
+      </c>
+      <c r="E5" s="1">
         <v>165697</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>194294</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>231633</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>202431</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>184577</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>141387</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>128899</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>112596</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>1262</v>
+      </c>
+      <c r="D6">
+        <v>126.38</v>
+      </c>
+      <c r="E6" s="1">
         <v>87960</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>131849</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>159767</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>179905</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>187853</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>184769</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>175951</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>160264</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1748</v>
+      </c>
+      <c r="D7">
+        <v>57.91</v>
+      </c>
+      <c r="E7" s="1">
         <v>87464</v>
       </c>
-      <c r="C7">
+      <c r="F7">
         <v>132581</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>143268</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>143019</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>129397</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>124467</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>115584</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>101661</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>2640</v>
+      </c>
+      <c r="D8">
+        <v>38.590000000000003</v>
+      </c>
+      <c r="E8" s="1">
         <v>84893</v>
       </c>
-      <c r="C8">
+      <c r="F8">
         <v>150825</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>173597</v>
       </c>
-      <c r="E8">
+      <c r="H8">
         <v>167599</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <v>144042</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>133084</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>119764</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>102295</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>3588</v>
+      </c>
+      <c r="D9">
+        <v>73.97</v>
+      </c>
+      <c r="E9" s="1">
         <v>165503</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>217653</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>237748</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>240621</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>323130</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>305505</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>296195</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>266503</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>5353</v>
+      </c>
+      <c r="D10">
+        <v>7.99</v>
+      </c>
+      <c r="E10" s="1">
         <v>155467</v>
       </c>
-      <c r="C10">
+      <c r="F10">
         <v>186871</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <v>172735</v>
       </c>
-      <c r="E10">
+      <c r="H10">
         <v>118329</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <v>85135</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>53677</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>50927</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>42893</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>2024</v>
+      </c>
+      <c r="D11">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="E11" s="1">
         <v>57107</v>
       </c>
-      <c r="C11">
+      <c r="F11">
         <v>90266</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>125049</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <v>127512</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>104625</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>93389</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>84836</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>70660</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>1823</v>
+      </c>
+      <c r="D12">
+        <v>35.15</v>
+      </c>
+      <c r="E12" s="1">
         <v>47877</v>
       </c>
-      <c r="C12">
+      <c r="F12">
         <v>79141</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>99657</v>
       </c>
-      <c r="E12">
+      <c r="H12">
         <v>99340</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>99334</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>85831</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>78034</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>64420</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <v>2030</v>
+      </c>
+      <c r="D13">
+        <v>64.17</v>
+      </c>
+      <c r="E13" s="1">
         <v>74136</v>
       </c>
-      <c r="C13">
+      <c r="F13">
         <v>99979</v>
       </c>
-      <c r="D13">
+      <c r="G13">
         <v>128790</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <v>154309</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>174998</v>
       </c>
-      <c r="G13">
+      <c r="J13">
         <v>176765</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>158575</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>130782</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>3646</v>
+      </c>
+      <c r="D14">
+        <v>43.82</v>
+      </c>
+      <c r="E14" s="1">
         <v>84091</v>
       </c>
-      <c r="C14">
+      <c r="F14">
         <v>123375</v>
       </c>
-      <c r="D14">
+      <c r="G14">
         <v>149855</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <v>174957</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>214777</v>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>162045</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>170017</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>160340</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>4155</v>
+      </c>
+      <c r="D15">
+        <v>62.1</v>
+      </c>
+      <c r="E15" s="1">
         <v>146505</v>
       </c>
-      <c r="C15">
+      <c r="F15">
         <v>209709</v>
       </c>
-      <c r="D15">
+      <c r="G15">
         <v>263024</v>
       </c>
-      <c r="E15">
+      <c r="H15">
         <v>328965</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <v>367193</v>
       </c>
-      <c r="G15">
+      <c r="J15">
         <v>330506</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>305032</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>259481</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>2994</v>
+      </c>
+      <c r="D16">
+        <v>32.19</v>
+      </c>
+      <c r="E16" s="1">
         <v>85163</v>
       </c>
-      <c r="C16">
+      <c r="F16">
         <v>118310</v>
       </c>
-      <c r="D16">
+      <c r="G16">
         <v>147166</v>
       </c>
-      <c r="E16">
+      <c r="H16">
         <v>164757</v>
       </c>
-      <c r="F16">
+      <c r="I16">
         <v>152477</v>
       </c>
-      <c r="G16">
+      <c r="J16">
         <v>112891</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>109375</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>96624</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>2454</v>
+      </c>
+      <c r="D17">
+        <v>58.32</v>
+      </c>
+      <c r="E17" s="1">
         <v>86768</v>
       </c>
-      <c r="C17">
+      <c r="F17">
         <v>125569</v>
       </c>
-      <c r="D17">
+      <c r="G17">
         <v>139340</v>
       </c>
-      <c r="E17">
+      <c r="H17">
         <v>193224</v>
       </c>
-      <c r="F17">
+      <c r="I17">
         <v>231241</v>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>204768</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>179521</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>144438</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>14045</v>
+      </c>
+      <c r="D18">
+        <v>93.26</v>
+      </c>
+      <c r="E18" s="1">
         <v>164242</v>
       </c>
-      <c r="C18">
+      <c r="F18">
         <v>249867</v>
       </c>
-      <c r="D18">
+      <c r="G18">
         <v>292321</v>
       </c>
-      <c r="E18">
+      <c r="H18">
         <v>339686</v>
       </c>
-      <c r="F18">
+      <c r="I18">
         <v>474019</v>
       </c>
-      <c r="G18">
+      <c r="J18">
         <v>463676</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>454798</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>425412</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19">
+        <v>2813</v>
+      </c>
+      <c r="D19">
+        <v>69.41</v>
+      </c>
+      <c r="E19" s="1">
         <v>117719</v>
       </c>
-      <c r="C19">
+      <c r="F19">
         <v>194455</v>
       </c>
-      <c r="D19">
+      <c r="G19">
         <v>223949</v>
       </c>
-      <c r="E19">
+      <c r="H19">
         <v>176838</v>
       </c>
-      <c r="F19">
+      <c r="I19">
         <v>204346</v>
       </c>
-      <c r="G19">
+      <c r="J19">
         <v>206344</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>208055</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>195794</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>1781</v>
+      </c>
+      <c r="D20">
+        <v>64.89</v>
+      </c>
+      <c r="E20" s="1">
         <v>63379</v>
       </c>
-      <c r="C20">
+      <c r="F20">
         <v>83135</v>
       </c>
-      <c r="D20">
+      <c r="G20">
         <v>90577</v>
       </c>
-      <c r="E20">
+      <c r="H20">
         <v>99593</v>
       </c>
-      <c r="F20">
+      <c r="I20">
         <v>126329</v>
       </c>
-      <c r="G20">
+      <c r="J20">
         <v>122870</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>122568</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>115862</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21">
+        <v>729</v>
+      </c>
+      <c r="D21">
+        <v>144.38</v>
+      </c>
+      <c r="E21" s="1">
         <v>55412</v>
       </c>
-      <c r="C21">
+      <c r="F21">
         <v>79808</v>
       </c>
-      <c r="D21">
+      <c r="G21">
         <v>99346</v>
       </c>
-      <c r="E21">
+      <c r="H21">
         <v>112073</v>
       </c>
-      <c r="F21">
+      <c r="I21">
         <v>119866</v>
       </c>
-      <c r="G21">
+      <c r="J21">
         <v>118426</v>
       </c>
-      <c r="H21">
+      <c r="K21">
         <v>113804</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>105863</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>641.20000000000005</v>
+      </c>
+      <c r="D22">
+        <v>1196</v>
+      </c>
+      <c r="E22" s="1">
         <v>48266</v>
       </c>
-      <c r="C22">
+      <c r="F22">
         <v>111565</v>
       </c>
-      <c r="D22">
+      <c r="G22">
         <v>258024</v>
       </c>
-      <c r="E22">
+      <c r="H22">
         <v>478076</v>
       </c>
-      <c r="F22">
+      <c r="I22">
         <v>777826</v>
       </c>
-      <c r="G22">
+      <c r="J22">
         <v>779145</v>
       </c>
-      <c r="H22">
+      <c r="K22">
         <v>790017</v>
       </c>
-      <c r="I22">
+      <c r="L22">
         <v>769944</v>
       </c>
     </row>

</xml_diff>